<commit_message>
Added additional search filters
I think im done :)
</commit_message>
<xml_diff>
--- a/hour_log.xlsx
+++ b/hour_log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sven\Desktop\DTT assessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sven\Desktop\DTT_assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C30952B-0D6C-46F6-B6D6-62481272414B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8530A97D-C791-43BA-8ACE-DB5F062826FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <r>
       <rPr>
@@ -141,13 +141,25 @@
     <t>Refactored the code to follow the Single Responsibility Principle (Added services used in the controller)</t>
   </si>
   <si>
-    <t>I didn't really looked into "SRP" (Signle responsibilty protocol) when i saw it mentioned in the assessment, but when i went through the checklist i saw it come by, i decided to look into it. This turned out to be a very time consuming choice because it took alot of time to refactor the code. I added a new services method with 2 services. These are then used in the controller. This way the, for example, the methods that validate input become reusable and more maintainable. I added a __construct in the FacilityController to initiate the DB connection and creating instances of the services, which then get the $db variable injected. I have seen code being structured like this but i never really understood why it was now.</t>
-  </si>
-  <si>
     <t>After looking through the assessment exercise, i think i have done everything it asked me in the best way i could</t>
   </si>
   <si>
     <t>I made sure to check all requirements set in the assessment. There might be some things that could be better regarding the SOLID design principle, performance/efficiency, PSR standards and ofcourse all the bonius features besides the version control using git. I know a little bit about unit testing, but im not experienced enough to apply that on the current API. I am satisfied with what i have build and i hope its up to your guys standards at DTT. I learned an incredible amount of new information/ways to code, which im really happy about.</t>
+  </si>
+  <si>
+    <t>After reading through the assessment once more, i decided to try to add another optional feature, the pagination for read operations. I have never done this before so i looked up some tutorials on the internet about it. I used this blog (https://www.merge.dev/blog/rest-api-pagination) and AI to understand how pagination works and how to implement it. After a while i could not figure out how to make it work so i went back to the way it was. I need to know pagination better before using it in a pretty complex API like this one. I did add some additional search filters to the search operation though!</t>
+  </si>
+  <si>
+    <t>I decided to try to add pagnation for the read operations and added new search filters to the search operation</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>I think im ready to finish this assessment. I spent 3 days working on this assessment as much and hard as i could. I believe i included all requirements and did everything that needed to be done for the assessment. I had an absolute blast making this thing, because i enjoyed learning / making something that i know will be important to do with my eyes closed in the future. I have learned a lot of new things, which im very excited about. Thank you guys.</t>
+  </si>
+  <si>
+    <t>I didn't really looked into "SRP" (Signle responsibilty protocol) when i saw it mentioned in the assessment, but when i went through the checklist i saw it come by, i decided to look into it. This turned out to be a very time consuming choice because it took alot of time to refactor the code. I found this website (https://medium.com/@Omojunior11/single-responsibility-principle-srp-example-using-php-337e33d739e) very usefull for understanding the basics. I added a new services method with 2 services. These are then used in the controller. This way the, for example, the methods that validate input become reusable and more maintainable. I added a __construct in the FacilityController to initiate the DB connection and creating instances of the services, which then get the $db variable injected. I have seen code being structured like this but i never really understood why it was now.</t>
   </si>
 </sst>
 </file>
@@ -876,7 +888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1095,14 +1107,14 @@
         <v>45774</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="39.75" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="17">
         <v>1</v>
@@ -1111,24 +1123,40 @@
         <v>45775</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="16"/>
+    <row r="16" spans="1:6" ht="39.75" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="17">
+        <v>1</v>
+      </c>
+      <c r="C16" s="18">
+        <v>45776</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="16"/>
+      <c r="A17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="18">
+        <v>45776</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="4"/>
     </row>
@@ -1234,7 +1262,7 @@
       </c>
       <c r="B30" s="11">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>18.5</v>
+        <v>19.5</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -1270,11 +1298,14 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:F2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D16" r:id="rId1" display="https://youtu.be/KrHkOzJxhss" xr:uid="{683ACE6B-75EF-4951-8DD4-927AF5381E28}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Arial,Regular"&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First batch of fixes after the feedback
- Altered the postman (i might be missing some stuff, but ill check once im done)
- The fetch now returns the tags as an array instead of a string
- I removed the hardcoded port. I hope this is all i have to change regarding the database part of the application.
- removed unnessecery search filters
- added documentation to the router page (I hope this is what y'all meant)
</commit_message>
<xml_diff>
--- a/hour_log.xlsx
+++ b/hour_log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sven\Desktop\DTT_assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99C82B3-3AEF-4461-A6D8-F882A9256CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBF2852-AE31-44EA-B9B4-64415EF22844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <r>
       <rPr>
@@ -160,6 +160,24 @@
   </si>
   <si>
     <t>I managed to make search API calls work with a single parameter like: key=city and value=Amsterdam. I tried adding multiple parameter support but I have not succeeded yet. I'm going to try that later. I'm happy for now. Looking back on the 25th, I have picked up so much new knowledge already. I'm really happy with what i've built so far.</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>I just got my feedback on the assessment and i got some good improvements to work on. Since i handed in the first version of the assessment, i have worked on a big project where i made the API and the fetch functionaily, on a greater level then this assessment. So i have learned alot of new things that i can improve.</t>
+  </si>
+  <si>
+    <t>Analyzed the feedback</t>
+  </si>
+  <si>
+    <t>I took a while to read through the feedback and made a clear scheme of what to improve. Im going to improve them one at a time. About the feedback about the search functionality, i got this feedback: "Search facilities allows me to search on each field but that is not what the assingment states." But in the assessment, it says "I want to be able to search facilities by the facility name, tag name, or location city, or any combination of those in a single API call." I misunderstood this part whoopsie. Its a pretty easy fix luckily. The tags are the cause of the most issue so thats where the most time will be spent probably.</t>
+  </si>
+  <si>
+    <t>Fixed the first couple issues</t>
+  </si>
+  <si>
+    <t>I started with some of the easier fixes like the unnessecery search filters, made the tagets return as an array and fixed the database port issue. I also added documentation to the router page. Im going to add example bodys in the postman collection aswell to make it even more clear. Next up will probably be all the tags issues.</t>
   </si>
 </sst>
 </file>
@@ -894,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1182,7 +1200,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>
@@ -1190,27 +1208,51 @@
       <c r="E20" s="7"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="16"/>
+    <row r="21" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="17">
+        <v>0</v>
+      </c>
+      <c r="C21" s="18">
+        <v>45796</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>36</v>
+      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="16"/>
+    <row r="22" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
+      <c r="A22" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="17">
+        <v>0</v>
+      </c>
+      <c r="C22" s="18">
+        <v>45796</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>38</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="16"/>
+    <row r="23" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A23" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="17">
+        <v>2</v>
+      </c>
+      <c r="C23" s="18">
+        <v>45796</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>40</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="4"/>
     </row>
@@ -1268,7 +1310,7 @@
       </c>
       <c r="B30" s="11">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>19.5</v>
+        <v>21.5</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>

</xml_diff>

<commit_message>
Feedback fixes batch 2
- Isolated the tag related code in FacilityService to TagService
- When searching with a tag filter, all tags of the found facilities are returned, not just the one you were looking for +the tags are returned as an array.
</commit_message>
<xml_diff>
--- a/hour_log.xlsx
+++ b/hour_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sven\Desktop\DTT_assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBF2852-AE31-44EA-B9B4-64415EF22844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B135D0EE-6DC8-495D-B1B7-3C7CC9085403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <r>
       <rPr>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>I started with some of the easier fixes like the unnessecery search filters, made the tagets return as an array and fixed the database port issue. I also added documentation to the router page. Im going to add example bodys in the postman collection aswell to make it even more clear. Next up will probably be all the tags issues.</t>
+  </si>
+  <si>
+    <t>Feedback fix batch 2</t>
+  </si>
+  <si>
+    <t>I started with creating a new service, the tagService, and putting the tag related stuff from facility service in there. This was very simple to do. Then i fixed the issue where, when searching with a filter for tags, the API would only return the tag you were looking for, not the other tags that were part of the facilities you fetched. Its also being returned as an array, so i think the tags in a string issue is returned everywhere now.</t>
   </si>
 </sst>
 </file>
@@ -404,7 +410,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -457,6 +463,9 @@
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -913,7 +922,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1256,11 +1265,19 @@
       <c r="E23" s="7"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="5"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="6"/>
+    <row r="24" spans="1:6" ht="39.75" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="17">
+        <v>1</v>
+      </c>
+      <c r="C24" s="18">
+        <v>45796</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>42</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="4"/>
     </row>
@@ -1310,7 +1327,7 @@
       </c>
       <c r="B30" s="11">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>21.5</v>
+        <v>22.5</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>

</xml_diff>

<commit_message>
Added models for the database data (its not being used yet)
</commit_message>
<xml_diff>
--- a/hour_log.xlsx
+++ b/hour_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sven\Desktop\DTT_assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B135D0EE-6DC8-495D-B1B7-3C7CC9085403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFF8607-663A-46AB-A02F-59F8B26AE95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <r>
       <rPr>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>I started with creating a new service, the tagService, and putting the tag related stuff from facility service in there. This was very simple to do. Then i fixed the issue where, when searching with a filter for tags, the API would only return the tag you were looking for, not the other tags that were part of the facilities you fetched. Its also being returned as an array, so i think the tags in a string issue is returned everywhere now.</t>
+  </si>
+  <si>
+    <t>Adding models for the database attempt no. 1</t>
+  </si>
+  <si>
+    <t>I had never heard or thought about using models. I visited this site (https://leafphp.dev/docs/database/models) to learn more. Now, i get the point of using models, and i made the model pages, but i dont really understand how to implement it yet. Ill try again later. First im going to try to add functionality to be able to add new tags.</t>
   </si>
 </sst>
 </file>
@@ -458,14 +464,14 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -922,34 +928,34 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.796875" customWidth="1"/>
+    <col min="1" max="1" width="26.296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.796875" customWidth="1"/>
     <col min="3" max="3" width="8.59765625" customWidth="1"/>
     <col min="4" max="4" width="79.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -1275,17 +1281,25 @@
       <c r="C24" s="18">
         <v>45796</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="23" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="5"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="6"/>
+    <row r="25" spans="1:6" ht="39.75" x14ac:dyDescent="0.35">
+      <c r="A25" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="17">
+        <v>1</v>
+      </c>
+      <c r="C25" s="18">
+        <v>45796</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="E25" s="7"/>
       <c r="F25" s="4"/>
     </row>
@@ -1293,7 +1307,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="17"/>
       <c r="C26" s="18"/>
-      <c r="D26" s="6"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="7"/>
       <c r="F26" s="4"/>
     </row>
@@ -1327,7 +1341,7 @@
       </c>
       <c r="B30" s="11">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>22.5</v>
+        <v>23.5</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>

</xml_diff>

<commit_message>
Fixed all the feedback regarding tags
-- Switched all the tags_id param with the tag names so you can now create new tags.
-- Added a new validation method for validating the facility id params.
-- Added more documentation
-- Updated the postman collection accordingly
</commit_message>
<xml_diff>
--- a/hour_log.xlsx
+++ b/hour_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sven\Desktop\DTT_assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFF8607-663A-46AB-A02F-59F8B26AE95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B964C314-8BD2-4982-ACE9-618496EB46B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <r>
       <rPr>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>I had never heard or thought about using models. I visited this site (https://leafphp.dev/docs/database/models) to learn more. Now, i get the point of using models, and i made the model pages, but i dont really understand how to implement it yet. Ill try again later. First im going to try to add functionality to be able to add new tags.</t>
+  </si>
+  <si>
+    <t>Fixed tag issues</t>
+  </si>
+  <si>
+    <t>I started off by switching out the tag_id params for tagName params, since it would not be possible to create tags when just passing tag ID's. So now you just pass in tag names, if the tag already exists, it will add that tag, and if it doesnt it will add the tag to the tags in the DB and add it to the facility. I also added validation checks for new tags to check if a string is given and to check if its not an empty string. I aslo added a validateFacilityId method to not write duplicate code. This all took me longer then expected but oh well. The only thing left, besides the bonus stuff, is the use of the model thingies. Im going to try my best to understand how to implement this. im going to continue tomorrow since its getting late haha.</t>
   </si>
 </sst>
 </file>
@@ -927,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1055,7 +1061,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>21</v>
       </c>
@@ -1303,11 +1309,19 @@
       <c r="E25" s="7"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="5"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="23"/>
+    <row r="26" spans="1:6" ht="65.25" x14ac:dyDescent="0.35">
+      <c r="A26" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="17">
+        <v>3</v>
+      </c>
+      <c r="C26" s="18">
+        <v>45796</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="E26" s="7"/>
       <c r="F26" s="4"/>
     </row>
@@ -1341,7 +1355,7 @@
       </c>
       <c r="B30" s="11">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>23.5</v>
+        <v>26.5</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>

</xml_diff>